<commit_message>
bill invoice -> credit purchase and product import bugfix
</commit_message>
<xml_diff>
--- a/public/uploads/media/default/sample_items.xlsx
+++ b/public/uploads/media/default/sample_items.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sahaf\Desktop\Mohamed\Sahafintech\ekstrabooks\public\uploads\media\default\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sahaf\Desktop\Mohamed\Sahafintech\ekstrabooks-v2.0\public\uploads\media\default\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4CFA187-1881-4D99-AF99-77D1C3F89DD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4577D7E-F216-4D42-8CFD-D3BE896533BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{3D70032A-A14A-4146-81AC-7DD5D2E1BEA5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3D70032A-A14A-4146-81AC-7DD5D2E1BEA5}"/>
   </bookViews>
   <sheets>
     <sheet name="sample_items" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>name</t>
   </si>
@@ -116,10 +116,13 @@
     <t>China</t>
   </si>
   <si>
-    <t>intial_stock</t>
-  </si>
-  <si>
     <t>sub_category</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>initial_stock</t>
   </si>
 </sst>
 </file>
@@ -501,142 +504,145 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8582DF61-F897-4B3E-8020-C8FC0D08B8D3}">
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.08984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.36328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.36328125" customWidth="1"/>
-    <col min="8" max="8" width="17.26953125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.36328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.26953125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.81640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.36328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.42578125" customWidth="1"/>
+    <col min="9" max="9" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="1" t="s">
+      <c r="S1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1">
+        <v>27</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="1">
         <v>10</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="N1" t="s">
-        <v>18</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="1">
-        <v>9</v>
-      </c>
-      <c r="E2" s="1">
-        <v>27</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="1">
-        <v>10</v>
-      </c>
-      <c r="H2" s="1">
-        <v>1</v>
       </c>
       <c r="I2" s="1">
         <v>1</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" s="1">
+        <v>1</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K2" s="1">
+      <c r="L2" s="1">
         <v>1</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="M2" s="1">
+      <c r="N2" s="1">
         <v>1</v>
       </c>
-      <c r="N2" s="2">
+      <c r="O2" s="2">
         <v>45467</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="P2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>22</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>24</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>